<commit_message>
bezier curves???? echt een gedrocht voorlopig
</commit_message>
<xml_diff>
--- a/Python/Nalox1_18_07_2018.xlsx
+++ b/Python/Nalox1_18_07_2018.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AA1"/>
+  <dimension ref="A1:AI1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -532,14 +532,14 @@
           <t>Transverse8</t>
         </is>
       </c>
-      <c r="P1" s="3" t="inlineStr">
-        <is>
-          <t>Descending9</t>
-        </is>
-      </c>
-      <c r="Q1" s="3" t="inlineStr">
-        <is>
-          <t>Descending10</t>
+      <c r="P1" s="2" t="inlineStr">
+        <is>
+          <t>Transverse9</t>
+        </is>
+      </c>
+      <c r="Q1" s="2" t="inlineStr">
+        <is>
+          <t>Transverse10</t>
         </is>
       </c>
       <c r="R1" s="3" t="inlineStr">
@@ -547,19 +547,19 @@
           <t>Descending11</t>
         </is>
       </c>
-      <c r="S1" s="4" t="inlineStr">
-        <is>
-          <t>Sigmoid12</t>
-        </is>
-      </c>
-      <c r="T1" s="4" t="inlineStr">
-        <is>
-          <t>Sigmoid13</t>
-        </is>
-      </c>
-      <c r="U1" s="4" t="inlineStr">
-        <is>
-          <t>Sigmoid14</t>
+      <c r="S1" s="3" t="inlineStr">
+        <is>
+          <t>Descending12</t>
+        </is>
+      </c>
+      <c r="T1" s="3" t="inlineStr">
+        <is>
+          <t>Descending13</t>
+        </is>
+      </c>
+      <c r="U1" s="3" t="inlineStr">
+        <is>
+          <t>Descending14</t>
         </is>
       </c>
       <c r="V1" s="4" t="inlineStr">
@@ -567,29 +567,69 @@
           <t>Sigmoid15</t>
         </is>
       </c>
-      <c r="W1" s="5" t="inlineStr">
-        <is>
-          <t>Rectum16</t>
-        </is>
-      </c>
-      <c r="X1" s="5" t="inlineStr">
-        <is>
-          <t>Rectum17</t>
-        </is>
-      </c>
-      <c r="Y1" s="5" t="inlineStr">
-        <is>
-          <t>Rectum18</t>
-        </is>
-      </c>
-      <c r="Z1" s="5" t="inlineStr">
-        <is>
-          <t>Rectum19</t>
-        </is>
-      </c>
-      <c r="AA1" s="5" t="inlineStr">
-        <is>
-          <t>Rectum20</t>
+      <c r="W1" s="4" t="inlineStr">
+        <is>
+          <t>Sigmoid16</t>
+        </is>
+      </c>
+      <c r="X1" s="4" t="inlineStr">
+        <is>
+          <t>Sigmoid17</t>
+        </is>
+      </c>
+      <c r="Y1" s="4" t="inlineStr">
+        <is>
+          <t>Sigmoid18</t>
+        </is>
+      </c>
+      <c r="Z1" s="4" t="inlineStr">
+        <is>
+          <t>Sigmoid19</t>
+        </is>
+      </c>
+      <c r="AA1" s="4" t="inlineStr">
+        <is>
+          <t>Sigmoid20</t>
+        </is>
+      </c>
+      <c r="AB1" s="4" t="inlineStr">
+        <is>
+          <t>Sigmoid21</t>
+        </is>
+      </c>
+      <c r="AC1" s="4" t="inlineStr">
+        <is>
+          <t>Sigmoid22</t>
+        </is>
+      </c>
+      <c r="AD1" s="4" t="inlineStr">
+        <is>
+          <t>Sigmoid23</t>
+        </is>
+      </c>
+      <c r="AE1" s="5" t="inlineStr">
+        <is>
+          <t>Rectum24</t>
+        </is>
+      </c>
+      <c r="AF1" s="5" t="inlineStr">
+        <is>
+          <t>Rectum25</t>
+        </is>
+      </c>
+      <c r="AG1" s="5" t="inlineStr">
+        <is>
+          <t>Rectum26</t>
+        </is>
+      </c>
+      <c r="AH1" s="5" t="inlineStr">
+        <is>
+          <t>Rectum27</t>
+        </is>
+      </c>
+      <c r="AI1" s="5" t="inlineStr">
+        <is>
+          <t>Rectum28</t>
         </is>
       </c>
     </row>

</xml_diff>